<commit_message>
add eigen toepassing and Quality notebooks
</commit_message>
<xml_diff>
--- a/notebook_overview.xlsx
+++ b/notebook_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onno__000\Documents\04_mamba\03_cursusmateriaal\raw_material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7D3F7F6C-C127-4862-A744-DE3CB9207107}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8ACD2CBA-69EC-428D-98D6-972CA950B287}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Notebook name</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>Syntax: for-statement</t>
+  </si>
+  <si>
+    <t>eigen_toepassing</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>creating coding blocks, think about goal, in- and output of code</t>
+  </si>
+  <si>
+    <t>Opdrachten toevoegen voor cursusdag 2 t/m 4</t>
   </si>
 </sst>
 </file>
@@ -1020,13 +1032,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1151,7 @@
         <v>29</v>
       </c>
       <c r="C5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -1165,7 +1177,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
@@ -1214,7 +1226,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
@@ -1227,6 +1239,29 @@
       </c>
       <c r="H8" s="2" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished ZEN of Python Notebook
</commit_message>
<xml_diff>
--- a/notebook_overview.xlsx
+++ b/notebook_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onno__000\Documents\04_mamba\03_cursusmateriaal\raw_material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8ACD2CBA-69EC-428D-98D6-972CA950B287}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F2E43271-44FA-49E9-9933-AAE234D60A98}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Notebook name</t>
   </si>
@@ -187,6 +187,24 @@
   </si>
   <si>
     <t>Opdrachten toevoegen voor cursusdag 2 t/m 4</t>
+  </si>
+  <si>
+    <t>code quality</t>
+  </si>
+  <si>
+    <t>afmaken</t>
+  </si>
+  <si>
+    <t>common_pitfalls.ipynb</t>
+  </si>
+  <si>
+    <t>Quality_ZEN_of_Python.ipynb</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>the ZEN of Python</t>
   </si>
 </sst>
 </file>
@@ -1032,13 +1050,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1100,7 +1118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1195,7 +1213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1218,7 +1236,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1262,6 +1280,46 @@
       </c>
       <c r="H9" s="2" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data processing examples
</commit_message>
<xml_diff>
--- a/notebook_overview.xlsx
+++ b/notebook_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\onno__000\Documents\04_mamba\03_cursusmateriaal\raw_material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7130B64E-789F-4B38-993B-AD06D4DDFD3F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AECB74DB-D5F3-42CE-A157-33074CC54EF5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Notebook name</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>pandas, plots, wordcloud</t>
+  </si>
+  <si>
+    <t>groundwater_model</t>
+  </si>
+  <si>
+    <t>flopy,  animation</t>
   </si>
 </sst>
 </file>
@@ -1071,13 +1077,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,6 +1389,26 @@
         <v>48</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I8" xr:uid="{9BB88C17-8B91-4E47-A536-010FCD44B292}">
     <filterColumn colId="1">

</xml_diff>